<commit_message>
Edits for status of transfer report
</commit_message>
<xml_diff>
--- a/exports/LGR5 niche quantification.xlsx
+++ b/exports/LGR5 niche quantification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work cache\py_projs\scRNAseq_AGR2\exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B8ED18-C892-447E-869A-D35982BAC88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E697892C-F03F-4362-92FD-909F12DF68F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{03385140-70EB-440F-94E9-26322C3D0E3A}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="16920" activeTab="1" xr2:uid="{03385140-70EB-440F-94E9-26322C3D0E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -138,14 +138,16 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -300,7 +302,7 @@
                   <c:v>4.5699999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14419999999999999</c:v>
+                  <c:v>0.1444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1548,15 +1550,15 @@
       <selection activeCell="A2" sqref="A2:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1570,15 +1572,15 @@
         <v>45428</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1589,7 +1591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1603,7 +1605,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1616,15 +1618,15 @@
         <v>5.6655665566556657E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -1635,7 +1637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1649,7 +1651,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1662,15 +1664,15 @@
         <v>0.16559485530546625</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -1681,7 +1683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1695,7 +1697,7 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1708,15 +1710,15 @@
         <v>0.11358368103847936</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -1727,7 +1729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1741,7 +1743,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1754,7 +1756,7 @@
         <v>0.27721335268505082</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
@@ -1768,15 +1770,15 @@
         <v>45428</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>0</v>
       </c>
@@ -1787,7 +1789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -1801,7 +1803,7 @@
         <v>4983</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1814,15 +1816,15 @@
         <v>0.29981938591210117</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>0</v>
       </c>
@@ -1833,7 +1835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -1847,7 +1849,7 @@
         <v>16289</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1879,21 +1881,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC11011-2BE0-44AA-B719-A01DB4490469}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="9" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1904,15 +1909,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C3">
-        <v>103</v>
+        <v>265</v>
       </c>
       <c r="D3">
         <v>1818</v>
@@ -1924,7 +1929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1934,31 +1939,34 @@
       <c r="C4">
         <v>5.6655665566556657E-2</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="2">
         <v>4.5699999999999998E-2</v>
       </c>
-      <c r="J4" s="5">
-        <v>0.14419999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="J4" s="2">
+        <v>0.1444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="2">
         <v>0.13500000000000001</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="2">
         <v>0.12870000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -1969,12 +1977,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C7">
         <v>103</v>
@@ -1983,7 +1991,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1994,12 +2002,15 @@
         <v>0.16559485530546625</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -2010,12 +2021,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13">
-        <v>311</v>
+        <v>352</v>
       </c>
       <c r="C13">
         <v>245</v>
@@ -2024,7 +2035,7 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -2035,12 +2046,15 @@
         <v>0.11358368103847936</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -2051,12 +2065,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
       <c r="B17">
-        <v>266</v>
+        <v>324</v>
       </c>
       <c r="C17">
         <v>573</v>
@@ -2065,7 +2079,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -2077,6 +2091,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A15:D15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>